<commit_message>
Enhance filtering functionality by adding tag support and updating filter logic
</commit_message>
<xml_diff>
--- a/Mappa_nodi.xlsx
+++ b/Mappa_nodi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://camozzicloud-my.sharepoint.com/personal/mpasseri_fonderiemoragavardo_it/Documents/Documenti/VSCode/EnergyMeters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="531" documentId="11_CBF82CE5D29271A855494D68F3BC070891C844B4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0348118-84DB-44A8-8DD2-2D8AB6EE1251}"/>
+  <xr:revisionPtr revIDLastSave="536" documentId="11_CBF82CE5D29271A855494D68F3BC070891C844B4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43BF1E3A-5F43-461F-980B-018DC74DA75E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="213" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="191" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="182">
   <si>
     <t>Cabina</t>
   </si>
@@ -657,7 +657,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -815,8 +815,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -834,6 +837,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1126,9 +1133,9 @@
   </sheetPr>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J7" sqref="J7"/>
+      <selection pane="topRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,7 +1146,7 @@
     <col min="4" max="4" width="23.7265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="9.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
     <col min="8" max="8" width="22.7265625" customWidth="1"/>
     <col min="9" max="9" width="14.7265625" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
@@ -1687,13 +1694,17 @@
       <c r="D20" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="4">
         <v>35</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="27"/>
+      <c r="H20" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20" s="35">
+        <v>10000</v>
+      </c>
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10" ht="58" x14ac:dyDescent="0.35">

</xml_diff>